<commit_message>
changes made on tiles
</commit_message>
<xml_diff>
--- a/tiles.xlsx
+++ b/tiles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Attom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20867533-7E24-422A-AD19-4CEE18F1D06E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A8E6D7-4F7A-40FD-90B0-79CD41BCEB2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="225">
   <si>
     <t>Keyword</t>
   </si>
@@ -692,6 +692,9 @@
   </si>
   <si>
     <t>dr fixit</t>
+  </si>
+  <si>
+    <t>stick on</t>
   </si>
 </sst>
 </file>
@@ -1057,10 +1060,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C216"/>
+  <dimension ref="A1:C221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="C216" sqref="C216"/>
+    <sheetView tabSelected="1" topLeftCell="A202" workbookViewId="0">
+      <selection activeCell="B221" sqref="B221"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1614,7 +1617,7 @@
         <v>70</v>
       </c>
       <c r="C61" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
@@ -2957,6 +2960,46 @@
       </c>
       <c r="C216" t="s">
         <v>216</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A217" t="s">
+        <v>224</v>
+      </c>
+      <c r="C217" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A218" t="s">
+        <v>4</v>
+      </c>
+      <c r="C218" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A219" t="s">
+        <v>110</v>
+      </c>
+      <c r="C219" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A220" t="s">
+        <v>80</v>
+      </c>
+      <c r="C220" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A221" t="s">
+        <v>84</v>
+      </c>
+      <c r="C221" t="s">
+        <v>221</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes made in tiles
</commit_message>
<xml_diff>
--- a/tiles.xlsx
+++ b/tiles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Attom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A8E6D7-4F7A-40FD-90B0-79CD41BCEB2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84990BB6-50DA-4333-A4DA-831531088008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="804" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="225">
   <si>
     <t>Keyword</t>
   </si>
@@ -1060,10 +1060,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C221"/>
+  <dimension ref="A1:C222"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A202" workbookViewId="0">
-      <selection activeCell="B221" sqref="B221"/>
+    <sheetView tabSelected="1" topLeftCell="A209" workbookViewId="0">
+      <selection activeCell="C222" sqref="C222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3002,6 +3002,14 @@
         <v>221</v>
       </c>
     </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A222" t="s">
+        <v>98</v>
+      </c>
+      <c r="C222" t="s">
+        <v>221</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>